<commit_message>
save changes made and delete registered animals
</commit_message>
<xml_diff>
--- a/dados_animais.xlsx
+++ b/dados_animais.xlsx
@@ -506,7 +506,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>SYNC_20240929102012.png</t>
+          <t>SYNC_20240930143148.png</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -522,13 +522,13 @@
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>POLVO</t>
+          <t>OCTOPUS</t>
         </is>
       </c>
       <c r="G2" t="inlineStr"/>
       <c r="H2" t="inlineStr">
         <is>
-          <t>LUCAS</t>
+          <t>BITBUILDERS</t>
         </is>
       </c>
       <c r="I2" t="inlineStr"/>
@@ -537,7 +537,7 @@
       <c r="L2" t="inlineStr"/>
       <c r="M2" t="inlineStr">
         <is>
-          <t>29/09/2024 - 10:20</t>
+          <t>30/09/2024 - 14:31</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
bug fixes for deleting the animal
</commit_message>
<xml_diff>
--- a/dados_animais.xlsx
+++ b/dados_animais.xlsx
@@ -506,7 +506,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>SYNC_20240930143148.png</t>
+          <t>SYNC_20240930192523.png</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -537,7 +537,7 @@
       <c r="L2" t="inlineStr"/>
       <c r="M2" t="inlineStr">
         <is>
-          <t>30/09/2024 - 14:31</t>
+          <t>30/09/2024 - 19:25</t>
         </is>
       </c>
     </row>

</xml_diff>